<commit_message>
Introduction Harmizert in Excel
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4661624-A6D9-4448-ABE6-949E611EF1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4444EFC6-71ED-274D-BCAA-C03B92CF9F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="780" windowWidth="28040" windowHeight="17360" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Objecten" sheetId="1" r:id="rId1"/>
+    <sheet name="Put" sheetId="2" r:id="rId2"/>
+    <sheet name="Spoor" sheetId="3" r:id="rId3"/>
+    <sheet name="Bot" sheetId="7" r:id="rId4"/>
+    <sheet name="Stelling" sheetId="5" r:id="rId5"/>
+    <sheet name="Artefact" sheetId="4" r:id="rId6"/>
+    <sheet name="Vondst" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="120">
   <si>
     <t>Tekening</t>
   </si>
@@ -45,106 +51,355 @@
     <t>Ignore</t>
   </si>
   <si>
-    <t>.*backup.*</t>
-  </si>
-  <si>
-    <t>TEKENING.*</t>
-  </si>
-  <si>
-    <t>VONDSTENLIJST, VONDST</t>
-  </si>
-  <si>
-    <t>HOUT</t>
-  </si>
-  <si>
     <t>Leer</t>
   </si>
   <si>
     <t>Hout</t>
   </si>
   <si>
-    <t>LEER</t>
-  </si>
-  <si>
     <t>Kleipijp</t>
   </si>
   <si>
     <t>Spoor</t>
   </si>
   <si>
-    <t>SPOREN, SPOOR</t>
-  </si>
-  <si>
     <t>Vulling</t>
   </si>
   <si>
-    <t>VULLING.*</t>
-  </si>
-  <si>
     <t>Steen</t>
   </si>
   <si>
-    <t>STEEN</t>
-  </si>
-  <si>
     <t>Glas</t>
   </si>
   <si>
     <t>Metaal</t>
   </si>
   <si>
-    <t>METAAL</t>
-  </si>
-  <si>
     <t>Dia</t>
   </si>
   <si>
-    <t>DIA.*</t>
-  </si>
-  <si>
     <t>Munt</t>
   </si>
   <si>
-    <t>MUNT.*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aardewerk </t>
-  </si>
-  <si>
-    <t>KLEIPIJPEN, ARTF_PIJP</t>
-  </si>
-  <si>
     <t>Skelet</t>
   </si>
   <si>
-    <t>Skelet.*</t>
-  </si>
-  <si>
     <t>Spijker</t>
   </si>
   <si>
-    <t>SPIJKER.*</t>
-  </si>
-  <si>
-    <t>GLAS, ARTF_GLS</t>
-  </si>
-  <si>
     <t>Foto</t>
   </si>
   <si>
-    <t>FOTO.*</t>
-  </si>
-  <si>
     <t>Put</t>
   </si>
   <si>
-    <t>PUT.*</t>
-  </si>
-  <si>
     <t>Artefact</t>
   </si>
   <si>
-    <t>ARTEFACT.*</t>
+    <t>["VONDSTENLIJST", "VONDST", "VONDSTINHD"]</t>
+  </si>
+  <si>
+    <t>["PUT", "PUTTEN"]</t>
+  </si>
+  <si>
+    <t>["HOUT"]</t>
+  </si>
+  <si>
+    <t>["LEER"]</t>
+  </si>
+  <si>
+    <t>["KLEIPIJPEN", "ARTF_PIJP"]</t>
+  </si>
+  <si>
+    <t>["STEEN"]</t>
+  </si>
+  <si>
+    <t>["GLAS", "ARTF_GLS"]</t>
+  </si>
+  <si>
+    <t>["METAAL"]</t>
+  </si>
+  <si>
+    <t>putnr</t>
+  </si>
+  <si>
+    <t>vlaknr</t>
+  </si>
+  <si>
+    <t>spoornr</t>
+  </si>
+  <si>
+    <t>["PUT", "PUTNO"]</t>
+  </si>
+  <si>
+    <t>Kolommen</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>["VLAK", "VLAKNO"]</t>
+  </si>
+  <si>
+    <t>["SPOOR", "SPOORNO"]</t>
+  </si>
+  <si>
+    <t>Tabellen</t>
+  </si>
+  <si>
+    <t>["SPOREN", "SPOOR"]</t>
+  </si>
+  <si>
+    <t>[".*backup.*", ".*kopie.*"]</t>
+  </si>
+  <si>
+    <t>["TEKENING.*"]</t>
+  </si>
+  <si>
+    <t>["VULLING.*"]</t>
+  </si>
+  <si>
+    <t>["DIA.*"]</t>
+  </si>
+  <si>
+    <t>["FOTO.*"]</t>
+  </si>
+  <si>
+    <t>["Skelet.*"]</t>
+  </si>
+  <si>
+    <t>["SPIJKER.*"]</t>
+  </si>
+  <si>
+    <t>["MUNT.*"]</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Aardewerk</t>
+  </si>
+  <si>
+    <t>stelling</t>
+  </si>
+  <si>
+    <t>["Stelling"]</t>
+  </si>
+  <si>
+    <t>inhoud</t>
+  </si>
+  <si>
+    <t>["inhoud"]</t>
+  </si>
+  <si>
+    <t>vondstnr</t>
+  </si>
+  <si>
+    <t>["VONDSTNO", "Vondst"]</t>
+  </si>
+  <si>
+    <t>doosnr</t>
+  </si>
+  <si>
+    <t>["DOOSNO", "10a"]</t>
+  </si>
+  <si>
+    <t>datering</t>
+  </si>
+  <si>
+    <t>["3", "1c", "DATERING"]</t>
+  </si>
+  <si>
+    <t>artefactnr</t>
+  </si>
+  <si>
+    <t>["SUBNO"]</t>
+  </si>
+  <si>
+    <t>beschrijving</t>
+  </si>
+  <si>
+    <t>["4b"]</t>
+  </si>
+  <si>
+    <t>["1b"]</t>
+  </si>
+  <si>
+    <t>dateringvanaf</t>
+  </si>
+  <si>
+    <t>["3a"]</t>
+  </si>
+  <si>
+    <t>dateringtot</t>
+  </si>
+  <si>
+    <t>["3b"]</t>
+  </si>
+  <si>
+    <t>typecd</t>
+  </si>
+  <si>
+    <t>["2"]</t>
+  </si>
+  <si>
+    <t>opmerkingen</t>
+  </si>
+  <si>
+    <t>["OPMERKING"]</t>
+  </si>
+  <si>
+    <t>typevoorwerp</t>
+  </si>
+  <si>
+    <t>["7a"]</t>
+  </si>
+  <si>
+    <t>functievoorwerp</t>
+  </si>
+  <si>
+    <t>["7b"]</t>
+  </si>
+  <si>
+    <t>origine</t>
+  </si>
+  <si>
+    <t>["8"]</t>
+  </si>
+  <si>
+    <t>literatuur</t>
+  </si>
+  <si>
+    <t>["9"]</t>
+  </si>
+  <si>
+    <t>tekeningnr</t>
+  </si>
+  <si>
+    <t>["10b"]</t>
+  </si>
+  <si>
+    <t>fotonr</t>
+  </si>
+  <si>
+    <t>["10d"]</t>
+  </si>
+  <si>
+    <t>dianr</t>
+  </si>
+  <si>
+    <t>["10c"]</t>
+  </si>
+  <si>
+    <t>restauratie</t>
+  </si>
+  <si>
+    <t>["12"]</t>
+  </si>
+  <si>
+    <t>exposabel</t>
+  </si>
+  <si>
+    <t>["13"]</t>
+  </si>
+  <si>
+    <t>conserveren</t>
+  </si>
+  <si>
+    <t>["14"]</t>
+  </si>
+  <si>
+    <t>["ARTEFACT.*", ".*AARDEWERK.*", ".*steen.*", ".*hout.*", ".*glas.*", ".*leer.*", ".*metaal.*", ".*munt.*", ".*spijker.*", ".*kleipijp.*", ".*bot.*", ".*skelet.*", ".*muur.*"]</t>
+  </si>
+  <si>
+    <t>lengte</t>
+  </si>
+  <si>
+    <t>["LENGTE"]</t>
+  </si>
+  <si>
+    <t>breedte</t>
+  </si>
+  <si>
+    <t>["BREEDTE"]</t>
+  </si>
+  <si>
+    <t>diepte</t>
+  </si>
+  <si>
+    <t>["DIEPTE"]</t>
+  </si>
+  <si>
+    <t>omstandigheden</t>
+  </si>
+  <si>
+    <t>["VONDSTOMSTH"]</t>
+  </si>
+  <si>
+    <t>["INHOUD"]</t>
+  </si>
+  <si>
+    <t>["VOORLOPIGEDATERING"]</t>
+  </si>
+  <si>
+    <t>xcoor_rd</t>
+  </si>
+  <si>
+    <t>["XCOORD"]</t>
+  </si>
+  <si>
+    <t>ycoor_rd</t>
+  </si>
+  <si>
+    <t>["YCOORD"]</t>
+  </si>
+  <si>
+    <t>datum</t>
+  </si>
+  <si>
+    <t>["DATUM"]</t>
+  </si>
+  <si>
+    <t>[".*AARDEWERK.*", "AW1.*"]</t>
+  </si>
+  <si>
+    <t>Keramiek</t>
+  </si>
+  <si>
+    <t>["ARTF_KER", "KERAMIEK.*"]</t>
+  </si>
+  <si>
+    <t>Bot</t>
+  </si>
+  <si>
+    <t>["ARTF_BOT"]</t>
+  </si>
+  <si>
+    <t>Overerven</t>
+  </si>
+  <si>
+    <t>Samenvoegen</t>
+  </si>
+  <si>
+    <t>publicatiecode</t>
+  </si>
+  <si>
+    <t>graf</t>
+  </si>
+  <si>
+    <t>["GRAF"]</t>
+  </si>
+  <si>
+    <t>Muur</t>
+  </si>
+  <si>
+    <t>["MUUR"]</t>
+  </si>
+  <si>
+    <t>["VLAK"]</t>
+  </si>
+  <si>
+    <t>Vlak</t>
   </si>
 </sst>
 </file>
@@ -496,164 +751,744 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795D4E60-F867-0244-8F0C-6B00236E8FA7}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="97.83203125" customWidth="1"/>
+    <col min="2" max="2" width="144.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC906335-C3CD-5343-8AF7-DDAC2E4E8FBD}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015E0221-97BC-C044-86E5-2C9D09B0EC27}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C77219-1328-B243-A5BB-B77D1DE9F3EF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EBFFEB-4950-BE4C-85B5-D39B5BCC4D46}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4001114-92A5-9946-8E19-4A561D8C734D}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E1AD00-9E44-2E49-9BA4-DA48C6654762}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge Artefacts toegevoegd: Cycle complete
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD018F5-D235-F84A-B05E-26D10636B0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B82D96-77E8-E14C-AEDC-35A8C813D349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="5" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="7" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Stelling" sheetId="5" r:id="rId5"/>
     <sheet name="Artefact" sheetId="4" r:id="rId6"/>
     <sheet name="Vondst" sheetId="6" r:id="rId7"/>
+    <sheet name="Glas" sheetId="8" r:id="rId8"/>
+    <sheet name="Hout" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="143">
   <si>
     <t>Tekening</t>
   </si>
@@ -216,9 +218,6 @@
     <t>beschrijving</t>
   </si>
   <si>
-    <t>["4b"]</t>
-  </si>
-  <si>
     <t>["1b"]</t>
   </si>
   <si>
@@ -249,15 +248,9 @@
     <t>typevoorwerp</t>
   </si>
   <si>
-    <t>["7a"]</t>
-  </si>
-  <si>
     <t>functievoorwerp</t>
   </si>
   <si>
-    <t>["7b"]</t>
-  </si>
-  <si>
     <t>origine</t>
   </si>
   <si>
@@ -267,15 +260,9 @@
     <t>literatuur</t>
   </si>
   <si>
-    <t>["9"]</t>
-  </si>
-  <si>
     <t>tekeningnr</t>
   </si>
   <si>
-    <t>["10b"]</t>
-  </si>
-  <si>
     <t>fotonr</t>
   </si>
   <si>
@@ -409,6 +396,81 @@
   </si>
   <si>
     <t>["SUBNO", "ARTEFACT", "ID"]</t>
+  </si>
+  <si>
+    <t>spooraard</t>
+  </si>
+  <si>
+    <t>["AARD"]</t>
+  </si>
+  <si>
+    <t>["BESCHRIJF"]</t>
+  </si>
+  <si>
+    <t>["DAT", "DATERING"]</t>
+  </si>
+  <si>
+    <t>["DOOSNR"]</t>
+  </si>
+  <si>
+    <t>glassoort</t>
+  </si>
+  <si>
+    <t>kleur</t>
+  </si>
+  <si>
+    <t>["kleur"]</t>
+  </si>
+  <si>
+    <t>decoratie</t>
+  </si>
+  <si>
+    <t>["decoratie"]</t>
+  </si>
+  <si>
+    <t>["4b", "BESCHR"]</t>
+  </si>
+  <si>
+    <t>["7b", "FUNCTIE"]</t>
+  </si>
+  <si>
+    <t>["9", "LITERATUUR"]</t>
+  </si>
+  <si>
+    <t>["10b", "TEKNO"]</t>
+  </si>
+  <si>
+    <t>["7a", "TYPE"]</t>
+  </si>
+  <si>
+    <t>maten</t>
+  </si>
+  <si>
+    <t>["4a"]</t>
+  </si>
+  <si>
+    <t>houtsoortcd</t>
+  </si>
+  <si>
+    <t>["5a"]</t>
+  </si>
+  <si>
+    <t>bewerkingssporen</t>
+  </si>
+  <si>
+    <t>["5b"]</t>
+  </si>
+  <si>
+    <t>gebruikssporen</t>
+  </si>
+  <si>
+    <t>["5b1"]</t>
+  </si>
+  <si>
+    <t>["5c"]</t>
+  </si>
+  <si>
+    <t>["glassoort", "GLSSOORT"]</t>
   </si>
 </sst>
 </file>
@@ -780,10 +842,10 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -852,10 +914,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -863,7 +925,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -937,7 +999,7 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -978,10 +1040,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -989,10 +1051,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1000,10 +1062,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -1011,10 +1073,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1024,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC906335-C3CD-5343-8AF7-DDAC2E4E8FBD}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,6 +1113,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1058,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015E0221-97BC-C044-86E5-2C9D09B0EC27}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1099,6 +1169,30 @@
       </c>
       <c r="B4" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1126,10 +1220,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1183,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4001114-92A5-9946-8E19-4A561D8C734D}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,7 +1348,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1262,127 +1356,127 @@
         <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
         <v>62</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
         <v>64</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1392,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E1AD00-9E44-2E49-9BA4-DA48C6654762}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1438,34 +1532,34 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1473,7 +1567,7 @@
         <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1481,31 +1575,31 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1513,7 +1607,131 @@
         <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BBA5D9-4EE3-3C49-A149-D0B6784307B3}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E4A0D3-C8F8-5044-BB56-6EEBE2D50DC8}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Bug with References and Keys
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD962A8-88AE-9A4A-A142-7B31BFA50B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72430AF2-5AFB-F642-8C27-2254AD7AB10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
   </bookViews>
@@ -476,7 +476,7 @@
     <t>["^VULLING.*"]</t>
   </si>
   <si>
-    <t>["^PUT$", "^PUTTEN$"]</t>
+    <t>["^PUT$", "PUTTEN"]</t>
   </si>
 </sst>
 </file>
@@ -831,7 +831,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Working Version (generated data nog added right)
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72430AF2-5AFB-F642-8C27-2254AD7AB10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2C99E0-E5DD-A54C-9EB6-F3F68D2D9F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
-    <sheet name="Put" sheetId="2" r:id="rId2"/>
-    <sheet name="Spoor" sheetId="3" r:id="rId3"/>
-    <sheet name="Bot" sheetId="7" r:id="rId4"/>
-    <sheet name="Stelling" sheetId="5" r:id="rId5"/>
-    <sheet name="Artefact" sheetId="4" r:id="rId6"/>
-    <sheet name="Vondst" sheetId="6" r:id="rId7"/>
-    <sheet name="Glas" sheetId="8" r:id="rId8"/>
-    <sheet name="Hout" sheetId="9" r:id="rId9"/>
+    <sheet name="Vlak" sheetId="10" r:id="rId2"/>
+    <sheet name="Put" sheetId="2" r:id="rId3"/>
+    <sheet name="Spoor" sheetId="3" r:id="rId4"/>
+    <sheet name="Bot" sheetId="7" r:id="rId5"/>
+    <sheet name="Stelling" sheetId="5" r:id="rId6"/>
+    <sheet name="Artefact" sheetId="4" r:id="rId7"/>
+    <sheet name="Vondst" sheetId="6" r:id="rId8"/>
+    <sheet name="Glas" sheetId="8" r:id="rId9"/>
+    <sheet name="Hout" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="145">
   <si>
     <t>Tekening</t>
   </si>
@@ -830,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795D4E60-F867-0244-8F0C-6B00236E8FA7}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1090,12 +1091,120 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E4A0D3-C8F8-5044-BB56-6EEBE2D50DC8}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65375499-C557-2047-BE48-517746E8A751}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC906335-C3CD-5343-8AF7-DDAC2E4E8FBD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1132,7 +1241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015E0221-97BC-C044-86E5-2C9D09B0EC27}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1222,7 +1331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C77219-1328-B243-A5BB-B77D1DE9F3EF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1253,7 +1362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EBFFEB-4950-BE4C-85B5-D39B5BCC4D46}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1295,7 +1404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4001114-92A5-9946-8E19-4A561D8C734D}">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -1506,7 +1615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E1AD00-9E44-2E49-9BA4-DA48C6654762}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -1645,7 +1754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BBA5D9-4EE3-3C49-A149-D0B6784307B3}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1693,70 +1802,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E4A0D3-C8F8-5044-BB56-6EEBE2D50DC8}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Recursief inlezen projecten uit DB en DC incl foto
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2C99E0-E5DD-A54C-9EB6-F3F68D2D9F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD69F77-38AB-0E49-B101-B23B57B3F835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="6" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
-    <sheet name="Vlak" sheetId="10" r:id="rId2"/>
-    <sheet name="Put" sheetId="2" r:id="rId3"/>
+    <sheet name="Put" sheetId="2" r:id="rId2"/>
+    <sheet name="Vlak" sheetId="10" r:id="rId3"/>
     <sheet name="Spoor" sheetId="3" r:id="rId4"/>
-    <sheet name="Bot" sheetId="7" r:id="rId5"/>
-    <sheet name="Stelling" sheetId="5" r:id="rId6"/>
+    <sheet name="Vulling" sheetId="11" r:id="rId5"/>
+    <sheet name="Vondst" sheetId="6" r:id="rId6"/>
     <sheet name="Artefact" sheetId="4" r:id="rId7"/>
-    <sheet name="Vondst" sheetId="6" r:id="rId8"/>
+    <sheet name="Bot" sheetId="7" r:id="rId8"/>
     <sheet name="Glas" sheetId="8" r:id="rId9"/>
     <sheet name="Hout" sheetId="9" r:id="rId10"/>
+    <sheet name="Stelling" sheetId="5" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="262">
   <si>
     <t>Tekening</t>
   </si>
@@ -306,9 +307,6 @@
     <t>["VONDSTOMSTH"]</t>
   </si>
   <si>
-    <t>["INHOUD"]</t>
-  </si>
-  <si>
     <t>["VOORLOPIGEDATERING"]</t>
   </si>
   <si>
@@ -360,12 +358,6 @@
     <t>["GRAF"]</t>
   </si>
   <si>
-    <t>Muur</t>
-  </si>
-  <si>
-    <t>["MUUR"]</t>
-  </si>
-  <si>
     <t>["VLAK"]</t>
   </si>
   <si>
@@ -381,12 +373,6 @@
     <t>["ARTEFACT.*"]</t>
   </si>
   <si>
-    <t>["AARD"]</t>
-  </si>
-  <si>
-    <t>["BESCHRIJF"]</t>
-  </si>
-  <si>
     <t>["DAT", "DATERING"]</t>
   </si>
   <si>
@@ -399,15 +385,9 @@
     <t>kleur</t>
   </si>
   <si>
-    <t>["kleur"]</t>
-  </si>
-  <si>
     <t>decoratie</t>
   </si>
   <si>
-    <t>["decoratie"]</t>
-  </si>
-  <si>
     <t>["4b", "BESCHR"]</t>
   </si>
   <si>
@@ -450,12 +430,6 @@
     <t>["5c"]</t>
   </si>
   <si>
-    <t>["glassoort", "GLSSOORT"]</t>
-  </si>
-  <si>
-    <t>["ARTEFACT", "SUBNO", "ID"]</t>
-  </si>
-  <si>
     <t>vorm</t>
   </si>
   <si>
@@ -474,10 +448,388 @@
     <t>["^SPOREN$", "^SPOOR$"]</t>
   </si>
   <si>
-    <t>["^VULLING.*"]</t>
-  </si>
-  <si>
     <t>["^PUT$", "PUTTEN"]</t>
+  </si>
+  <si>
+    <t>aangelegd</t>
+  </si>
+  <si>
+    <t>["AANGELEGD"]</t>
+  </si>
+  <si>
+    <t>["BESCHRYF"]</t>
+  </si>
+  <si>
+    <t>datum_aanleg</t>
+  </si>
+  <si>
+    <t>["DAT_AANLEG"]</t>
+  </si>
+  <si>
+    <t>vlaktype</t>
+  </si>
+  <si>
+    <t>["VTYPE"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is ook een systeemtabel voor komt uit SYS_LOOKUP </t>
+  </si>
+  <si>
+    <t>datum_ingevoerd</t>
+  </si>
+  <si>
+    <t>["INGEVOERD"]</t>
+  </si>
+  <si>
+    <t>datum_gewijzigd</t>
+  </si>
+  <si>
+    <t>["GEWIJZIGD"]</t>
+  </si>
+  <si>
+    <t>afgewerkt</t>
+  </si>
+  <si>
+    <t>["AFGEWERKT"]</t>
+  </si>
+  <si>
+    <t>breedte_bovenkant</t>
+  </si>
+  <si>
+    <t>breedte_onderkant</t>
+  </si>
+  <si>
+    <t>["BB"]</t>
+  </si>
+  <si>
+    <t>["BO"]</t>
+  </si>
+  <si>
+    <t>hoogte_bovenkant</t>
+  </si>
+  <si>
+    <t>["HB"]</t>
+  </si>
+  <si>
+    <t>hoogte_onderkant</t>
+  </si>
+  <si>
+    <t>["HO"]</t>
+  </si>
+  <si>
+    <t>["BESCHRIJVING"]</t>
+  </si>
+  <si>
+    <t>coupnrs</t>
+  </si>
+  <si>
+    <t>["COUPENR"]</t>
+  </si>
+  <si>
+    <t>Lijstje coupenummers maken</t>
+  </si>
+  <si>
+    <t>gecoupeerd</t>
+  </si>
+  <si>
+    <t>["GECOUPEERD"]</t>
+  </si>
+  <si>
+    <t>sporen_zelfde_periode</t>
+  </si>
+  <si>
+    <t>["GELIJKTIJDIG MET"]</t>
+  </si>
+  <si>
+    <t>identiek_aan</t>
+  </si>
+  <si>
+    <t>["IDENTIEK AAN"]</t>
+  </si>
+  <si>
+    <t>Is verwijzing</t>
+  </si>
+  <si>
+    <t>["AARD", "INTERPRET", "INTERPRETATIE"]</t>
+  </si>
+  <si>
+    <t>Relatie met SYS_LOOKUP sinterpret. We denken dat het ABR is</t>
+  </si>
+  <si>
+    <t>["JONGER DAN"]</t>
+  </si>
+  <si>
+    <t>jonger_dan</t>
+  </si>
+  <si>
+    <t>["LB"]</t>
+  </si>
+  <si>
+    <t>lengte_bovenkant</t>
+  </si>
+  <si>
+    <t>ouder_dan</t>
+  </si>
+  <si>
+    <t>["OUDER DAN"]</t>
+  </si>
+  <si>
+    <t>onderkant_NAP</t>
+  </si>
+  <si>
+    <t>["OK_NAP"]</t>
+  </si>
+  <si>
+    <t>profiel</t>
+  </si>
+  <si>
+    <t>["PROFIEL"]</t>
+  </si>
+  <si>
+    <t>richting_spoor</t>
+  </si>
+  <si>
+    <t>["RICHTING SPOOR"]</t>
+  </si>
+  <si>
+    <t>["STEENFORMAAT"]</t>
+  </si>
+  <si>
+    <t>Grootte baksteen, hoe groter hoe ouder</t>
+  </si>
+  <si>
+    <t>steenformaat</t>
+  </si>
+  <si>
+    <t>metselverband</t>
+  </si>
+  <si>
+    <t>["VERBANDEN (muur)"]</t>
+  </si>
+  <si>
+    <t>In RAAP zit ook nog een muurtabel</t>
+  </si>
+  <si>
+    <t>["INHOUD", "OPMERKING"]</t>
+  </si>
+  <si>
+    <t>segment</t>
+  </si>
+  <si>
+    <t>["SEGMENT"]</t>
+  </si>
+  <si>
+    <t>vaknummer</t>
+  </si>
+  <si>
+    <t>["VAKNR", "VAKLETTER"]</t>
+  </si>
+  <si>
+    <t>verzamelwijze</t>
+  </si>
+  <si>
+    <t>["VERZMWIJZE"]</t>
+  </si>
+  <si>
+    <t>RAAP komt uit SYS_LOOKUP vvverzamel</t>
+  </si>
+  <si>
+    <t>vullingnr</t>
+  </si>
+  <si>
+    <t>["VULLING"]</t>
+  </si>
+  <si>
+    <t>aantal</t>
+  </si>
+  <si>
+    <t>["AANTAL"]</t>
+  </si>
+  <si>
+    <t>subnr</t>
+  </si>
+  <si>
+    <t>["SUBNO"]</t>
+  </si>
+  <si>
+    <t>["VULLING", "VULLINGNO"]</t>
+  </si>
+  <si>
+    <t>["ARTEFACT", "ID", "SUBNO"]</t>
+  </si>
+  <si>
+    <t>In RAAP heb je zowel ARTEFACT en ook SUBNO. De Foto's worden gematcht op subnr. Uniek nummer in RAAP: ARTEFACT en SPLIT_ID</t>
+  </si>
+  <si>
+    <t>bioturbatie</t>
+  </si>
+  <si>
+    <t>["BIOTURB"]</t>
+  </si>
+  <si>
+    <t>["TEXTUUR"]</t>
+  </si>
+  <si>
+    <t>textuur</t>
+  </si>
+  <si>
+    <t>Is ook referentietabel voor</t>
+  </si>
+  <si>
+    <t>mediaan</t>
+  </si>
+  <si>
+    <t>["MEDIAAN"]</t>
+  </si>
+  <si>
+    <t>textuurbijmenging</t>
+  </si>
+  <si>
+    <t>["TBIJMENG"]</t>
+  </si>
+  <si>
+    <t>sublaag</t>
+  </si>
+  <si>
+    <t>["SUBLAAG"]</t>
+  </si>
+  <si>
+    <t>["KLEUR"]</t>
+  </si>
+  <si>
+    <t>reductie</t>
+  </si>
+  <si>
+    <t>["REDUCTIE"]</t>
+  </si>
+  <si>
+    <t>gevlekt</t>
+  </si>
+  <si>
+    <t>["GEVLEKT"]</t>
+  </si>
+  <si>
+    <t>Coderingen is SYS_LOOKUP vkleur</t>
+  </si>
+  <si>
+    <t>laaginterpretatie</t>
+  </si>
+  <si>
+    <t>["LGINTERP"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coderingen is SYS_LOOKUP </t>
+  </si>
+  <si>
+    <t>schelpenresten</t>
+  </si>
+  <si>
+    <t>["LSR"]</t>
+  </si>
+  <si>
+    <t>Zoek ook op meta-informatie bij tabel</t>
+  </si>
+  <si>
+    <t>grondsoort</t>
+  </si>
+  <si>
+    <t>["GRONDSOORT"]</t>
+  </si>
+  <si>
+    <t>lengte_baksteen1</t>
+  </si>
+  <si>
+    <t>["LB1"]</t>
+  </si>
+  <si>
+    <t>lengte_baksteen2</t>
+  </si>
+  <si>
+    <t>lengte_baksteen3</t>
+  </si>
+  <si>
+    <t>["LB2"]</t>
+  </si>
+  <si>
+    <t>["LB3"]</t>
+  </si>
+  <si>
+    <t>hoogte_baksteen1</t>
+  </si>
+  <si>
+    <t>hoogte_baksteen2</t>
+  </si>
+  <si>
+    <t>hoogte_baksteen3</t>
+  </si>
+  <si>
+    <t>["HB1"]</t>
+  </si>
+  <si>
+    <t>["HB2"]</t>
+  </si>
+  <si>
+    <t>["HB3"]</t>
+  </si>
+  <si>
+    <t>breedte_baksteen1</t>
+  </si>
+  <si>
+    <t>breedte_baksteen2</t>
+  </si>
+  <si>
+    <t>breedte_baksteen3</t>
+  </si>
+  <si>
+    <t>["BB1"]</t>
+  </si>
+  <si>
+    <t>["BB2"]</t>
+  </si>
+  <si>
+    <t>["BB3"]</t>
+  </si>
+  <si>
+    <t>De Muur-tabel samenvoegen in de Vullingtabel</t>
+  </si>
+  <si>
+    <t>["^VULLING.*", "MUUR"]</t>
+  </si>
+  <si>
+    <t>opmerking</t>
+  </si>
+  <si>
+    <t>minimum_aantal_individuen</t>
+  </si>
+  <si>
+    <t>past_aan_andere_nummers</t>
+  </si>
+  <si>
+    <t>["4d"]</t>
+  </si>
+  <si>
+    <t>["5a", "glassoort", "GLSSOORT"]</t>
+  </si>
+  <si>
+    <t>["5b", "kleur"]</t>
+  </si>
+  <si>
+    <t>["5c", "decoratie"]</t>
+  </si>
+  <si>
+    <t>["4c", "MAI"]</t>
+  </si>
+  <si>
+    <t>ABR-codering</t>
+  </si>
+  <si>
+    <t>["ABR"]</t>
+  </si>
+  <si>
+    <t>Zelf toevoeging</t>
+  </si>
+  <si>
+    <t>ABR-code</t>
   </si>
 </sst>
 </file>
@@ -829,19 +1181,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795D4E60-F867-0244-8F0C-6B00236E8FA7}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="144.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -849,13 +1201,16 @@
         <v>32</v>
       </c>
       <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -863,39 +1218,39 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -903,7 +1258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -911,31 +1266,31 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -946,7 +1301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -957,7 +1312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -968,7 +1323,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -979,7 +1334,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1006,7 +1361,7 @@
         <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1047,10 +1402,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
         <v>96</v>
-      </c>
-      <c r="B22" t="s">
-        <v>97</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1058,10 +1413,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
         <v>98</v>
-      </c>
-      <c r="B23" t="s">
-        <v>99</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1072,18 +1427,7 @@
         <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1114,42 +1458,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1157,212 +1501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65375499-C557-2047-BE48-517746E8A751}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC906335-C3CD-5343-8AF7-DDAC2E4E8FBD}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015E0221-97BC-C044-86E5-2C9D09B0EC27}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C77219-1328-B243-A5BB-B77D1DE9F3EF}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EBFFEB-4950-BE4C-85B5-D39B5BCC4D46}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1404,18 +1543,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4001114-92A5-9946-8E19-4A561D8C734D}">
-  <dimension ref="A1:B24"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC906335-C3CD-5343-8AF7-DDAC2E4E8FBD}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1436,178 +1575,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1615,12 +1610,580 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E1AD00-9E44-2E49-9BA4-DA48C6654762}">
-  <dimension ref="A1:B15"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65375499-C557-2047-BE48-517746E8A751}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015E0221-97BC-C044-86E5-2C9D09B0EC27}">
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053B96B0-00F3-9945-BF70-7BCDDD4A976D}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B17" t="s">
+        <v>231</v>
+      </c>
+      <c r="C17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>236</v>
+      </c>
+      <c r="B20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>237</v>
+      </c>
+      <c r="B21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>250</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E1AD00-9E44-2E49-9BA4-DA48C6654762}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1698,7 +2261,7 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1706,31 +2269,31 @@
         <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
         <v>89</v>
-      </c>
-      <c r="B11" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="s">
         <v>91</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
         <v>93</v>
-      </c>
-      <c r="B13" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1738,7 +2301,7 @@
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1746,7 +2309,314 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B18" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4001114-92A5-9946-8E19-4A561D8C734D}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C77219-1328-B243-A5BB-B77D1DE9F3EF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1756,14 +2626,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BBA5D9-4EE3-3C49-A149-D0B6784307B3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1777,26 +2648,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set unique for Vondst
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AE1A67-12C6-C94F-B53D-049EB1100AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBCB27D-097E-2C4A-B6E0-53823EAA004E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
   </bookViews>
@@ -385,9 +385,6 @@
     <t>["^TEKENING.*"]</t>
   </si>
   <si>
-    <t>["^VONDSTENLIJST", "^VONDST$"]</t>
-  </si>
-  <si>
     <t>["^SPOREN$", "^SPOOR$"]</t>
   </si>
   <si>
@@ -860,6 +857,9 @@
   </si>
   <si>
     <t>["3", "1c", "DATERING", "3datering voorwerp", "DAT_VRWP" ]</t>
+  </si>
+  <si>
+    <t>["^VONDSTENLIJST", "^VONDST$", "VONDSTINHD"]</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795D4E60-F867-0244-8F0C-6B00236E8FA7}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1238,7 @@
         <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1262,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1270,7 +1270,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1278,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1302,7 +1302,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1318,7 +1318,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -1329,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1351,7 +1351,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1373,7 +1373,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
@@ -1384,7 +1384,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" t="s">
         <v>247</v>
-      </c>
-      <c r="B18" t="s">
-        <v>248</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1439,7 +1439,7 @@
         <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1455,10 +1455,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>248</v>
+      </c>
+      <c r="B24" t="s">
         <v>249</v>
-      </c>
-      <c r="B24" t="s">
-        <v>250</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -1466,10 +1466,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" t="s">
         <v>251</v>
-      </c>
-      <c r="B25" t="s">
-        <v>252</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -1477,10 +1477,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B26" t="s">
         <v>253</v>
-      </c>
-      <c r="B26" t="s">
-        <v>254</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -1488,10 +1488,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" t="s">
         <v>255</v>
-      </c>
-      <c r="B27" t="s">
-        <v>256</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
@@ -1499,10 +1499,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28" t="s">
         <v>257</v>
-      </c>
-      <c r="B28" t="s">
-        <v>258</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
@@ -1656,31 +1656,31 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
         <v>116</v>
-      </c>
-      <c r="B4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
         <v>124</v>
-      </c>
-      <c r="B5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
         <v>126</v>
-      </c>
-      <c r="B6" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1732,26 +1732,26 @@
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
         <v>119</v>
-      </c>
-      <c r="B5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
         <v>121</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>122</v>
-      </c>
-      <c r="C6" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -1810,10 +1810,10 @@
         <v>111</v>
       </c>
       <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" t="s">
         <v>149</v>
-      </c>
-      <c r="C5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1821,7 +1821,7 @@
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1850,159 +1850,159 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" t="s">
         <v>128</v>
-      </c>
-      <c r="B10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
         <v>134</v>
-      </c>
-      <c r="B13" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" t="s">
         <v>136</v>
-      </c>
-      <c r="B14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" t="s">
         <v>139</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>140</v>
-      </c>
-      <c r="C16" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
         <v>142</v>
-      </c>
-      <c r="B17" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" t="s">
         <v>144</v>
       </c>
-      <c r="B18" t="s">
-        <v>145</v>
-      </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" t="s">
         <v>146</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>147</v>
-      </c>
-      <c r="C19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" t="s">
         <v>155</v>
       </c>
-      <c r="B21" t="s">
-        <v>156</v>
-      </c>
       <c r="C21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" t="s">
         <v>157</v>
-      </c>
-      <c r="B22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
         <v>159</v>
-      </c>
-      <c r="B23" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B25" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" t="s">
         <v>162</v>
-      </c>
-      <c r="C25" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" t="s">
         <v>165</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>166</v>
-      </c>
-      <c r="C26" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2043,10 +2043,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2067,45 +2067,45 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" t="s">
         <v>184</v>
-      </c>
-      <c r="B6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" t="s">
         <v>187</v>
-      </c>
-      <c r="B7" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" t="s">
         <v>189</v>
-      </c>
-      <c r="B8" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
         <v>191</v>
-      </c>
-      <c r="B9" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" t="s">
         <v>193</v>
-      </c>
-      <c r="B10" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2113,139 +2113,139 @@
         <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" t="s">
         <v>196</v>
-      </c>
-      <c r="B12" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" t="s">
         <v>198</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>199</v>
-      </c>
-      <c r="C13" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" t="s">
         <v>201</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>202</v>
-      </c>
-      <c r="C14" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" t="s">
         <v>204</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>205</v>
-      </c>
-      <c r="C15" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" t="s">
         <v>207</v>
-      </c>
-      <c r="B16" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" t="s">
         <v>209</v>
       </c>
-      <c r="B17" t="s">
-        <v>210</v>
-      </c>
       <c r="C17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
         <v>52</v>
@@ -2339,7 +2339,7 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2392,37 +2392,37 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" t="s">
         <v>169</v>
-      </c>
-      <c r="B16" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" t="s">
         <v>171</v>
-      </c>
-      <c r="B17" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" t="s">
         <v>173</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>174</v>
-      </c>
-      <c r="C18" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" t="s">
         <v>176</v>
-      </c>
-      <c r="B19" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2457,7 +2457,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2481,7 +2481,7 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2497,7 +2497,7 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2505,18 +2505,18 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
         <v>182</v>
-      </c>
-      <c r="C8" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
         <v>179</v>
-      </c>
-      <c r="B9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2524,7 +2524,7 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2532,7 +2532,7 @@
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2572,7 +2572,7 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2596,7 +2596,7 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2628,7 +2628,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2636,7 +2636,7 @@
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2644,26 +2644,26 @@
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" t="s">
         <v>237</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>238</v>
-      </c>
-      <c r="C27" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2729,7 +2729,7 @@
         <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2737,7 +2737,7 @@
         <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2745,23 +2745,23 @@
         <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" t="s">
         <v>231</v>
-      </c>
-      <c r="B6" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ook meta info van RAAP projecten gebruikt
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBCB27D-097E-2C4A-B6E0-53823EAA004E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEC7A32-7056-E84D-AD06-DE6AA65862FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
   </bookViews>
@@ -385,6 +385,9 @@
     <t>["^TEKENING.*"]</t>
   </si>
   <si>
+    <t>["^VONDSTENLIJST", "^VONDST$"]</t>
+  </si>
+  <si>
     <t>["^SPOREN$", "^SPOOR$"]</t>
   </si>
   <si>
@@ -857,9 +860,6 @@
   </si>
   <si>
     <t>["3", "1c", "DATERING", "3datering voorwerp", "DAT_VRWP" ]</t>
-  </si>
-  <si>
-    <t>["^VONDSTENLIJST", "^VONDST$", "VONDSTINHD"]</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1238,7 @@
         <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1262,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1270,7 +1270,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1278,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1302,7 +1302,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1318,7 +1318,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -1329,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1351,7 +1351,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1373,7 +1373,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
@@ -1384,7 +1384,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1439,7 +1439,7 @@
         <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1455,10 +1455,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B24" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -1466,10 +1466,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -1477,10 +1477,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B26" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -1488,10 +1488,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
@@ -1499,10 +1499,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B28" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
@@ -1656,31 +1656,31 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1732,26 +1732,26 @@
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -1810,10 +1810,10 @@
         <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1821,7 +1821,7 @@
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1850,159 +1850,159 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" t="s">
         <v>153</v>
-      </c>
-      <c r="B15" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" t="s">
         <v>151</v>
       </c>
-      <c r="B20" t="s">
-        <v>150</v>
-      </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" t="s">
         <v>163</v>
-      </c>
-      <c r="B25" t="s">
-        <v>161</v>
-      </c>
-      <c r="C25" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2043,10 +2043,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2067,45 +2067,45 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
         <v>186</v>
       </c>
-      <c r="B7" t="s">
-        <v>185</v>
-      </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2113,139 +2113,139 @@
         <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B20" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B26" t="s">
         <v>52</v>
@@ -2339,7 +2339,7 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2392,37 +2392,37 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2457,7 +2457,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2481,7 +2481,7 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2497,7 +2497,7 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2505,18 +2505,18 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2524,7 +2524,7 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2532,7 +2532,7 @@
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2572,7 +2572,7 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2596,7 +2596,7 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2628,7 +2628,7 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2636,7 +2636,7 @@
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2644,26 +2644,26 @@
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B27" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C27" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2729,7 +2729,7 @@
         <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2737,7 +2737,7 @@
         <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2745,23 +2745,23 @@
         <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix in docker files
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEC7A32-7056-E84D-AD06-DE6AA65862FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5836BE95-7753-C948-B554-17AD477D2585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="7" xr2:uid="{287C8D65-6B9D-2447-AC8C-82CE397A5B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="289">
   <si>
     <t>Tekening</t>
   </si>
@@ -169,9 +169,6 @@
     <t>doosnr</t>
   </si>
   <si>
-    <t>["DOOSNO", "10a"]</t>
-  </si>
-  <si>
     <t>datering</t>
   </si>
   <si>
@@ -844,9 +841,6 @@
     <t>["4b", "BESCHR", "4bvoorwerp beschrijving", "BESCHRYF"]</t>
   </si>
   <si>
-    <t>["9", "LITERATUUR", "9literatuur", "LITERA" ]</t>
-  </si>
-  <si>
     <t>["AANTAL", "TOTAANTAL"]</t>
   </si>
   <si>
@@ -860,6 +854,63 @@
   </si>
   <si>
     <t>["3", "1c", "DATERING", "3datering voorwerp", "DAT_VRWP" ]</t>
+  </si>
+  <si>
+    <t>afmeting</t>
+  </si>
+  <si>
+    <t>["AFMETING"]</t>
+  </si>
+  <si>
+    <t>associatie</t>
+  </si>
+  <si>
+    <t>["ASSOCIA"]</t>
+  </si>
+  <si>
+    <t>["BEWERKING"]</t>
+  </si>
+  <si>
+    <t>brandsporen</t>
+  </si>
+  <si>
+    <t>["BRAND"]</t>
+  </si>
+  <si>
+    <t>slijtage_onderkaaks_DP4</t>
+  </si>
+  <si>
+    <t>["DP4"]</t>
+  </si>
+  <si>
+    <t>skeletdeel</t>
+  </si>
+  <si>
+    <t>["ELEMENT"]</t>
+  </si>
+  <si>
+    <t>aantal_puzzelen</t>
+  </si>
+  <si>
+    <t>["FRAGM"]</t>
+  </si>
+  <si>
+    <t>geconserveerd</t>
+  </si>
+  <si>
+    <t>["GECONSERVEERD"]</t>
+  </si>
+  <si>
+    <t>gewicht</t>
+  </si>
+  <si>
+    <t>["GEWICHT"]</t>
+  </si>
+  <si>
+    <t>["DOOSNO", "10a", "DOOS_NO"]</t>
+  </si>
+  <si>
+    <t>["9", "LITERATUUR", "9literatuur", "LITERA", "Bibliografie", "LITERAT" ]</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795D4E60-F867-0244-8F0C-6B00236E8FA7}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1232,13 +1283,13 @@
         <v>27</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
       <c r="E1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1254,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1262,7 +1313,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1270,7 +1321,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1278,7 +1329,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1302,7 +1353,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1310,7 +1361,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1318,7 +1369,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -1329,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1351,7 +1402,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1373,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
@@ -1384,7 +1435,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1392,10 +1443,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" t="s">
         <v>247</v>
-      </c>
-      <c r="B18" t="s">
-        <v>248</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1425,10 +1476,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
         <v>81</v>
-      </c>
-      <c r="B21" t="s">
-        <v>82</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -1436,10 +1487,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1447,18 +1498,18 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>248</v>
+      </c>
+      <c r="B24" t="s">
         <v>249</v>
-      </c>
-      <c r="B24" t="s">
-        <v>250</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -1466,10 +1517,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" t="s">
         <v>251</v>
-      </c>
-      <c r="B25" t="s">
-        <v>252</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -1477,10 +1528,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B26" t="s">
         <v>253</v>
-      </c>
-      <c r="B26" t="s">
-        <v>254</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -1488,10 +1539,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" t="s">
         <v>255</v>
-      </c>
-      <c r="B27" t="s">
-        <v>256</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
@@ -1499,10 +1550,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28" t="s">
         <v>257</v>
-      </c>
-      <c r="B28" t="s">
-        <v>258</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
@@ -1536,42 +1587,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
         <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
         <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
         <v>104</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1653,34 +1704,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
         <v>116</v>
-      </c>
-      <c r="B4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
         <v>124</v>
-      </c>
-      <c r="B5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
         <v>126</v>
-      </c>
-      <c r="B6" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1729,29 +1780,29 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
         <v>119</v>
-      </c>
-      <c r="B5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
         <v>121</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>122</v>
-      </c>
-      <c r="C6" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1791,7 +1842,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -1807,202 +1858,202 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" t="s">
         <v>149</v>
-      </c>
-      <c r="C5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
         <v>109</v>
-      </c>
-      <c r="B8" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
         <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" t="s">
         <v>128</v>
-      </c>
-      <c r="B10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
         <v>134</v>
-      </c>
-      <c r="B13" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" t="s">
         <v>136</v>
-      </c>
-      <c r="B14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" t="s">
         <v>139</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>140</v>
-      </c>
-      <c r="C16" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
         <v>142</v>
-      </c>
-      <c r="B17" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" t="s">
         <v>144</v>
       </c>
-      <c r="B18" t="s">
-        <v>145</v>
-      </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" t="s">
         <v>146</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>147</v>
-      </c>
-      <c r="C19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" t="s">
         <v>155</v>
       </c>
-      <c r="B21" t="s">
-        <v>156</v>
-      </c>
       <c r="C21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" t="s">
         <v>157</v>
-      </c>
-      <c r="B22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
         <v>159</v>
-      </c>
-      <c r="B23" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B25" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" t="s">
         <v>162</v>
-      </c>
-      <c r="C25" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" t="s">
         <v>165</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>166</v>
-      </c>
-      <c r="C26" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2043,10 +2094,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2067,188 +2118,188 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" t="s">
         <v>184</v>
-      </c>
-      <c r="B6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" t="s">
         <v>187</v>
-      </c>
-      <c r="B7" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" t="s">
         <v>189</v>
-      </c>
-      <c r="B8" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
         <v>191</v>
-      </c>
-      <c r="B9" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" t="s">
         <v>193</v>
-      </c>
-      <c r="B10" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" t="s">
         <v>196</v>
-      </c>
-      <c r="B12" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" t="s">
         <v>198</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>199</v>
-      </c>
-      <c r="C13" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" t="s">
         <v>201</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>202</v>
-      </c>
-      <c r="C14" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" t="s">
         <v>204</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>205</v>
-      </c>
-      <c r="C15" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" t="s">
         <v>207</v>
-      </c>
-      <c r="B16" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" t="s">
         <v>209</v>
       </c>
-      <c r="B17" t="s">
-        <v>210</v>
-      </c>
       <c r="C17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2304,34 +2355,34 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
         <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
         <v>70</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
         <v>72</v>
-      </c>
-      <c r="B8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2339,39 +2390,39 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
         <v>75</v>
-      </c>
-      <c r="B11" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
         <v>77</v>
-      </c>
-      <c r="B12" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
         <v>79</v>
-      </c>
-      <c r="B13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2379,7 +2430,7 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2387,42 +2438,42 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" t="s">
         <v>169</v>
-      </c>
-      <c r="B16" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" t="s">
         <v>171</v>
-      </c>
-      <c r="B17" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" t="s">
         <v>173</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>174</v>
-      </c>
-      <c r="C18" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" t="s">
         <v>176</v>
-      </c>
-      <c r="B19" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2432,16 +2483,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4001114-92A5-9946-8E19-4A561D8C734D}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A3" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2457,7 +2508,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2481,7 +2532,7 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2489,181 +2540,189 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
         <v>182</v>
-      </c>
-      <c r="C8" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
         <v>179</v>
-      </c>
-      <c r="B9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
         <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
         <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
         <v>51</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" t="s">
         <v>237</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>238</v>
       </c>
-      <c r="C27" t="s">
-        <v>239</v>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>285</v>
+      </c>
+      <c r="B28" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2673,13 +2732,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C77219-1328-B243-A5BB-B77D1DE9F3EF}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2691,10 +2754,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
-        <v>88</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2726,42 +2853,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" t="s">
         <v>231</v>
-      </c>
-      <c r="B6" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging and moving improved
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44535F11-EC42-3A46-B710-763111AAD2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA41B8D-3418-6D47-889B-87689409399C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="597">
   <si>
     <t>Object</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Keramiek</t>
   </si>
   <si>
-    <t>["ARTF_KER", "KERAMIEK.*"]</t>
-  </si>
-  <si>
     <t>Bot</t>
   </si>
   <si>
@@ -628,9 +625,6 @@
     <t>vondstnr</t>
   </si>
   <si>
-    <t>["VONDST", "VONDSTNO"]</t>
-  </si>
-  <si>
     <t>doosnr</t>
   </si>
   <si>
@@ -691,12 +685,6 @@
     <t>artefactnr</t>
   </si>
   <si>
-    <t>['ARTEFACT', 'SUBNO', 'ID']</t>
-  </si>
-  <si>
-    <t>In RAAP heb je zowel ARTEFACT en ook SUBNO. De Foto's worden gematcht op subnr. Uniek nummer in RAAP: ARTEFACT en SPLIT_ID</t>
-  </si>
-  <si>
     <t>['4bvoorwerp beschrijving', '4b', 'BESCHR', 'VOORZIJDE BEELD', 'BYZONDER1', 'BYZONDER2', 'BESCHRYF']</t>
   </si>
   <si>
@@ -829,9 +817,6 @@
     <t>subnr</t>
   </si>
   <si>
-    <t>['SUBNO']</t>
-  </si>
-  <si>
     <t>tekeningnr</t>
   </si>
   <si>
@@ -1826,6 +1811,27 @@
   </si>
   <si>
     <t>['LITERAT', 'PUBL_CODE', 'LITERATUUR', 'LITERA', 'Bibliografie', '9literatuur', '9', 'BIBLIOGRAFIE', 'CATALOGI', 'BIBLIOGRAFIE']</t>
+  </si>
+  <si>
+    <t>splitid</t>
+  </si>
+  <si>
+    <t>['SPLIT_ID']</t>
+  </si>
+  <si>
+    <t>['SUBNO', 'SUB_NO', 'sub', 'subnr']</t>
+  </si>
+  <si>
+    <t>['ARTEFACT']</t>
+  </si>
+  <si>
+    <t>Uniek nummer exclusief voor RAAP-database In RAAP heb je zowel ARTEFACT en ook SUBNO. De Foto's worden gematcht op subnr. Uniek nummer in RAAP: ARTEFACT en SPLIT_ID</t>
+  </si>
+  <si>
+    <t>["ARTF_KER", "KERAMIEK$"]</t>
+  </si>
+  <si>
+    <t>["VONDST", "VONDSTNO", "Vondst I"]</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1861,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1878,13 +1884,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2191,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A14" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2468,7 +2488,7 @@
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>595</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -2479,10 +2499,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
         <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -2493,10 +2513,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
         <v>47</v>
-      </c>
-      <c r="C23" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2504,10 +2524,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
         <v>49</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
@@ -2518,10 +2538,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
         <v>51</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
@@ -2532,10 +2552,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
         <v>53</v>
-      </c>
-      <c r="C26" t="s">
-        <v>54</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
@@ -2546,10 +2566,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
         <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>56</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
@@ -2560,10 +2580,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
         <v>57</v>
-      </c>
-      <c r="C28" t="s">
-        <v>58</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
@@ -2591,13 +2611,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2605,10 +2625,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2616,10 +2636,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2627,10 +2647,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2638,10 +2658,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2649,10 +2669,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2660,10 +2680,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2671,10 +2691,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C8" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2682,10 +2702,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C9" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2693,10 +2713,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C10" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2704,10 +2724,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="C11" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2715,10 +2735,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C12" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2726,10 +2746,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C13" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2737,10 +2757,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2748,10 +2768,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C15" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2759,10 +2779,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C16" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2770,10 +2790,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C17" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -2798,13 +2818,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2812,10 +2832,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2823,10 +2843,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2834,10 +2854,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C4" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2845,10 +2865,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2856,10 +2876,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2867,10 +2887,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C7" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2878,10 +2898,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2889,10 +2909,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C9" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2900,10 +2920,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C10" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2926,13 +2946,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2940,10 +2960,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2951,10 +2971,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C3" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2962,10 +2982,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2973,10 +2993,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2984,10 +3004,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C6" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2995,10 +3015,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C7" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3006,10 +3026,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C8" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3017,10 +3037,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C9" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3028,10 +3048,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C10" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3039,10 +3059,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C11" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3050,10 +3070,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C12" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3061,10 +3081,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C13" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3072,10 +3092,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C14" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3083,10 +3103,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C15" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3094,10 +3114,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C16" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3105,10 +3125,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C17" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3116,10 +3136,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C18" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3127,10 +3147,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C19" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3138,10 +3158,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C20" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3149,10 +3169,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C21" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3160,10 +3180,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C22" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3171,10 +3191,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C23" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3182,10 +3202,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C24" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3193,10 +3213,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C25" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3204,10 +3224,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3219,7 +3239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3229,16 +3249,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3256,13 +3276,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3270,10 +3290,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3281,10 +3301,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3292,10 +3312,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3303,10 +3323,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C5" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3314,10 +3334,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3325,10 +3345,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C7" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3336,10 +3356,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C8" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3347,10 +3367,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C9" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3358,10 +3378,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C10" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3369,10 +3389,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C11" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -3390,13 +3410,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3414,13 +3434,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3428,10 +3448,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C2" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3439,10 +3459,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3450,10 +3470,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3461,10 +3481,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C5" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3472,10 +3492,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C6" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3483,10 +3503,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C7" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3494,10 +3514,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C8" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3505,10 +3525,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C9" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3516,10 +3536,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C10" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3527,10 +3547,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C11" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3538,10 +3558,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C12" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3549,10 +3569,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C13" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3560,10 +3580,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C14" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3571,10 +3591,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C15" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3582,10 +3602,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C16" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3593,10 +3613,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C17" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3604,10 +3624,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C18" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3615,10 +3635,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C19" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3626,10 +3646,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C20" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3637,10 +3657,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C21" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3648,10 +3668,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C22" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3659,10 +3679,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C23" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3670,10 +3690,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C24" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3681,10 +3701,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C25" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3692,10 +3712,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C26" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3703,10 +3723,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="C27" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3714,10 +3734,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C28" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3725,10 +3745,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="C29" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3736,10 +3756,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C30" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3763,13 +3783,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3777,10 +3797,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3788,10 +3808,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C3" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3799,10 +3819,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="C4" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3810,10 +3830,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3821,10 +3841,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C6" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3832,10 +3852,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C7" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3843,10 +3863,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C8" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3854,10 +3874,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C9" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3865,10 +3885,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C10" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3876,10 +3896,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3887,10 +3907,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C12" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3898,10 +3918,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C13" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3909,10 +3929,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C14" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3920,10 +3940,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C15" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3931,10 +3951,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3942,10 +3962,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C17" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3953,10 +3973,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C18" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3964,10 +3984,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C19" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3975,10 +3995,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C20" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3986,10 +4006,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C21" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3997,10 +4017,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C22" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4008,10 +4028,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C23" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4019,10 +4039,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C24" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4030,10 +4050,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C25" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4041,10 +4061,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C26" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4052,10 +4072,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C27" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4063,10 +4083,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -4088,13 +4108,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4102,10 +4122,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4113,10 +4133,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4124,10 +4144,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C4" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4135,10 +4155,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C5" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4146,10 +4166,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4157,10 +4177,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="C7" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4168,10 +4188,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C8" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4179,10 +4199,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C9" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4190,10 +4210,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C10" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4201,10 +4221,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4212,10 +4232,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C12" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4223,10 +4243,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C13" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4234,10 +4254,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C14" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4245,10 +4265,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="C15" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4256,10 +4276,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C16" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4267,10 +4287,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="C17" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4278,10 +4298,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="C18" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -4299,13 +4319,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4313,10 +4333,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="C2" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4324,10 +4344,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C3" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4335,10 +4355,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4346,10 +4366,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4357,10 +4377,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="C6" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4368,10 +4388,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C7" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4379,10 +4399,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C8" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4390,10 +4410,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C9" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4401,10 +4421,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C10" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4412,10 +4432,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C11" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4423,10 +4443,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="C12" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4434,10 +4454,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C13" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4445,10 +4465,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C14" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4456,10 +4476,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C15" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4467,10 +4487,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C16" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4478,10 +4498,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="C17" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -4503,10 +4523,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4514,10 +4534,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -4525,10 +4545,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
         <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4536,10 +4556,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -4547,10 +4567,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -4558,10 +4578,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
         <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -4579,13 +4599,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -4603,13 +4623,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4617,10 +4637,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4628,10 +4648,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C3" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4639,10 +4659,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C4" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4650,10 +4670,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C5" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4661,10 +4681,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C6" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4672,10 +4692,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="C7" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4683,10 +4703,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C8" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4694,10 +4714,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4705,10 +4725,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="C10" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4716,10 +4736,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C11" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4727,10 +4747,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4738,10 +4758,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="C13" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4749,10 +4769,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="C14" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4760,10 +4780,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="C15" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4771,10 +4791,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="C16" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4782,10 +4802,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C17" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4793,10 +4813,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C18" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -4804,10 +4824,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="C19" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -4815,10 +4835,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="C20" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -4826,10 +4846,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="C21" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -4837,10 +4857,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="C22" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4848,10 +4868,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="C23" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4859,10 +4879,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C24" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4870,10 +4890,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4881,10 +4901,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="C26" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -4906,13 +4926,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4920,10 +4940,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="C2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4931,10 +4951,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C3" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4942,10 +4962,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C4" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4953,10 +4973,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C5" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4964,10 +4984,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C6" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4975,10 +4995,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C7" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4986,10 +5006,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="C8" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4997,10 +5017,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C9" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5008,10 +5028,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C10" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5019,10 +5039,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="C11" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5030,10 +5050,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="C12" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5041,10 +5061,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="C13" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5052,10 +5072,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="C14" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5063,10 +5083,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="C15" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5074,10 +5094,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C16" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -5085,10 +5105,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="C17" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -5096,10 +5116,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="C18" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -5120,13 +5140,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5134,10 +5154,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5145,10 +5165,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5156,10 +5176,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
         <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5167,10 +5187,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
         <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5178,13 +5198,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
         <v>76</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>77</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -5207,13 +5227,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5221,10 +5241,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5232,10 +5252,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5243,10 +5263,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
         <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5254,13 +5274,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
         <v>82</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>83</v>
-      </c>
-      <c r="D5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5268,10 +5288,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -5279,10 +5299,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
         <v>86</v>
-      </c>
-      <c r="C7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5290,10 +5310,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
         <v>88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5301,10 +5321,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
         <v>90</v>
-      </c>
-      <c r="C9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5312,10 +5332,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
         <v>92</v>
-      </c>
-      <c r="C10" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5323,10 +5343,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
         <v>94</v>
-      </c>
-      <c r="C11" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5334,10 +5354,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
         <v>96</v>
-      </c>
-      <c r="C12" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5345,10 +5365,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
         <v>98</v>
-      </c>
-      <c r="C13" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5356,10 +5376,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
         <v>100</v>
-      </c>
-      <c r="C14" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5367,10 +5387,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" t="s">
         <v>102</v>
-      </c>
-      <c r="C15" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5378,13 +5398,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" t="s">
         <v>104</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>105</v>
-      </c>
-      <c r="D16" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -5392,10 +5412,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
         <v>107</v>
-      </c>
-      <c r="C17" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -5403,13 +5423,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
         <v>109</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>110</v>
-      </c>
-      <c r="D18" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -5417,13 +5437,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" t="s">
         <v>112</v>
       </c>
-      <c r="C19" t="s">
-        <v>113</v>
-      </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -5431,13 +5451,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" t="s">
         <v>114</v>
       </c>
-      <c r="C20" t="s">
-        <v>115</v>
-      </c>
       <c r="D20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -5445,13 +5465,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" t="s">
         <v>116</v>
       </c>
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -5459,10 +5479,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
         <v>118</v>
-      </c>
-      <c r="C22" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -5470,10 +5490,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" t="s">
         <v>120</v>
-      </c>
-      <c r="C23" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -5481,10 +5501,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" t="s">
         <v>122</v>
-      </c>
-      <c r="C24" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -5492,13 +5512,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" t="s">
         <v>124</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>125</v>
-      </c>
-      <c r="D25" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -5506,13 +5526,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
         <v>127</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>128</v>
-      </c>
-      <c r="D26" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -5534,13 +5554,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5548,10 +5568,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5559,10 +5579,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
         <v>130</v>
-      </c>
-      <c r="C3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5570,10 +5590,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
         <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5581,10 +5601,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
         <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5592,10 +5612,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
         <v>132</v>
-      </c>
-      <c r="C6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -5603,13 +5623,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
         <v>134</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>135</v>
-      </c>
-      <c r="D7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5617,10 +5637,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" t="s">
         <v>137</v>
-      </c>
-      <c r="C8" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5628,10 +5648,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" t="s">
         <v>139</v>
-      </c>
-      <c r="C9" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5639,10 +5659,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
         <v>141</v>
-      </c>
-      <c r="C10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5650,13 +5670,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" t="s">
         <v>143</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>144</v>
-      </c>
-      <c r="D11" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5664,10 +5684,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
         <v>146</v>
-      </c>
-      <c r="C12" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5675,13 +5695,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" t="s">
         <v>148</v>
       </c>
-      <c r="C13" t="s">
-        <v>149</v>
-      </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5689,13 +5709,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" t="s">
         <v>150</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>151</v>
-      </c>
-      <c r="D14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5703,13 +5723,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" t="s">
         <v>153</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>154</v>
-      </c>
-      <c r="D15" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5717,10 +5737,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" t="s">
         <v>156</v>
-      </c>
-      <c r="C16" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -5728,13 +5748,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" t="s">
         <v>158</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>159</v>
-      </c>
-      <c r="D17" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -5742,10 +5762,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
         <v>161</v>
-      </c>
-      <c r="C18" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -5753,10 +5773,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" t="s">
         <v>163</v>
-      </c>
-      <c r="C19" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -5764,10 +5784,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" t="s">
         <v>165</v>
-      </c>
-      <c r="C20" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -5775,10 +5795,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" t="s">
         <v>167</v>
-      </c>
-      <c r="C21" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -5786,10 +5806,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" t="s">
         <v>169</v>
-      </c>
-      <c r="C22" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -5797,10 +5817,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" t="s">
         <v>171</v>
-      </c>
-      <c r="C23" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -5808,10 +5828,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" t="s">
         <v>173</v>
-      </c>
-      <c r="C24" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -5819,10 +5839,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" t="s">
         <v>175</v>
-      </c>
-      <c r="C25" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -5830,10 +5850,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" t="s">
         <v>177</v>
-      </c>
-      <c r="C26" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5845,19 +5865,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5865,10 +5887,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5876,10 +5898,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5887,10 +5909,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
         <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5898,10 +5920,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" t="s">
         <v>179</v>
-      </c>
-      <c r="C5" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5909,10 +5931,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
         <v>181</v>
-      </c>
-      <c r="C6" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -5920,10 +5942,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
         <v>90</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5931,10 +5953,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
         <v>183</v>
-      </c>
-      <c r="C8" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5942,10 +5964,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" t="s">
         <v>185</v>
-      </c>
-      <c r="C9" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5953,10 +5975,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5964,10 +5986,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" t="s">
         <v>188</v>
-      </c>
-      <c r="C11" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5975,10 +5997,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" t="s">
         <v>190</v>
-      </c>
-      <c r="C12" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5986,10 +6008,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" t="s">
         <v>192</v>
-      </c>
-      <c r="C13" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5997,10 +6019,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>596</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6008,10 +6030,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -6019,10 +6041,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -6030,10 +6052,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -6041,13 +6063,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" t="s">
         <v>202</v>
-      </c>
-      <c r="C18" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -6055,10 +6077,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -6076,10 +6098,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -6087,10 +6109,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -6098,10 +6120,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -6111,10 +6133,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6126,13 +6148,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6140,13 +6162,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6154,10 +6176,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6165,10 +6187,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6176,10 +6198,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="C5" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6187,10 +6209,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="C6" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6198,13 +6220,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>593</v>
       </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6212,10 +6234,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6223,10 +6245,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6234,10 +6256,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C10" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6245,10 +6267,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6256,10 +6278,10 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6267,10 +6289,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C13" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6278,10 +6300,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C14" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6289,10 +6311,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C15" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -6300,10 +6322,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -6311,10 +6333,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -6322,10 +6344,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C18" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -6333,10 +6355,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C19" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -6344,10 +6366,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -6355,10 +6377,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C21" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -6366,10 +6388,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C22" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -6377,10 +6399,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C23" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -6388,19 +6410,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="C24" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="C25" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -6408,10 +6430,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C26" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -6419,10 +6441,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C27" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -6430,10 +6452,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C28" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -6441,10 +6463,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C29" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -6452,10 +6474,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C30" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -6463,10 +6485,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -6474,10 +6496,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C32" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -6485,10 +6507,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -6496,10 +6518,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C34" t="s">
-        <v>262</v>
+        <v>592</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -6507,10 +6529,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C35" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -6518,10 +6540,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C36" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -6529,10 +6551,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C37" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -6540,10 +6562,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C38" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -6551,10 +6573,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -6562,10 +6584,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -6573,10 +6595,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C41" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -6584,10 +6606,21 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C42" t="s">
-        <v>274</v>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>590</v>
+      </c>
+      <c r="C43" t="s">
+        <v>591</v>
       </c>
     </row>
   </sheetData>
@@ -6605,13 +6638,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import photos and dia's
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_Harmonize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA41B8D-3418-6D47-889B-87689409399C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36C7E44-346B-C24A-8407-6C7D700B9EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="6" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,15 @@
     <sheet name="Ivoor" sheetId="20" r:id="rId20"/>
     <sheet name="Keramiek" sheetId="21" r:id="rId21"/>
     <sheet name="Leer" sheetId="22" r:id="rId22"/>
+    <sheet name="Fotobeschrijving" sheetId="23" r:id="rId23"/>
+    <sheet name="Fotokoppel" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="618">
   <si>
     <t>Object</t>
   </si>
@@ -1832,6 +1834,69 @@
   </si>
   <si>
     <t>["VONDST", "VONDSTNO", "Vondst I"]</t>
+  </si>
+  <si>
+    <t>Fotobeschrijving</t>
+  </si>
+  <si>
+    <t>["DIAOPGRAVING", "DIAVOORWERP", "Fotolijst"]</t>
+  </si>
+  <si>
+    <t>bestandsnaam</t>
+  </si>
+  <si>
+    <t>["Bestandsnaam"]</t>
+  </si>
+  <si>
+    <t>["Datum"]</t>
+  </si>
+  <si>
+    <t>omschrijving</t>
+  </si>
+  <si>
+    <t>["Omschrijving"]</t>
+  </si>
+  <si>
+    <t>["SPOORNO"]</t>
+  </si>
+  <si>
+    <t>["Vlak"]</t>
+  </si>
+  <si>
+    <t>["Richting"]</t>
+  </si>
+  <si>
+    <t>pad</t>
+  </si>
+  <si>
+    <t>["PAD"]</t>
+  </si>
+  <si>
+    <t>["SUBNO"]</t>
+  </si>
+  <si>
+    <t>["VONDSTNO"]</t>
+  </si>
+  <si>
+    <t>["Foto Totaal Tabel"]</t>
+  </si>
+  <si>
+    <t>["A-B-C-D Nr's"]</t>
+  </si>
+  <si>
+    <t>materiaalgroep</t>
+  </si>
+  <si>
+    <t>["Materiaalgroep"]</t>
+  </si>
+  <si>
+    <t>["Nieuwe Bestandsnaam"]</t>
+  </si>
+  <si>
+    <t>Fotokoppel</t>
+  </si>
+  <si>
+    <t>abcd-nr</t>
   </si>
 </sst>
 </file>
@@ -2209,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A10" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2587,6 +2652,28 @@
       </c>
       <c r="D28" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>597</v>
+      </c>
+      <c r="C29" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>616</v>
+      </c>
+      <c r="C30" t="s">
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -4916,7 +5003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5124,6 +5213,179 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC0267F-3961-F64D-889C-497261B556CC}">
+  <dimension ref="B1:D12"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C2" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>602</v>
+      </c>
+      <c r="C4" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>607</v>
+      </c>
+      <c r="C9" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" t="s">
+        <v>610</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D0D174-6E0A-4C40-A400-825ECAC5A597}">
+  <dimension ref="B1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>613</v>
+      </c>
+      <c r="C3" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5865,7 +6127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>